<commit_message>
upload TEST EXECUTION regist 2
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CE70D8-B192-4531-8E72-4D227F17BC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD67BAB-1FE6-466A-9024-154D307076B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>SUB</t>
   </si>
@@ -111,6 +111,24 @@
   </si>
   <si>
     <t>Verify system prevents duplicate email registration</t>
+  </si>
+  <si>
+    <t>Register using already registered email</t>
+  </si>
+  <si>
+    <t>Error message appears</t>
+  </si>
+  <si>
+    <t>Error message “Email already registered” displayed</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>BUG-01</t>
   </si>
 </sst>
 </file>
@@ -145,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +191,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -226,6 +250,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -544,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A298028-139E-4333-8689-0C2300BF2C53}">
   <dimension ref="D4:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -558,7 +585,8 @@
     <col min="8" max="8" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="21" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="21" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21" style="6" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="6"/>
@@ -669,28 +697,28 @@
         <v>24</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="P6" s="7">
-        <v>46077</v>
+        <v>46076</v>
       </c>
       <c r="Q6" s="5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
update TEST EXCETUION regist 3
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD67BAB-1FE6-466A-9024-154D307076B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F67A43C-4CBC-49A7-B5C0-79A086074F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>SUB</t>
   </si>
@@ -129,6 +129,25 @@
   </si>
   <si>
     <t>BUG-01</t>
+  </si>
+  <si>
+    <t>EXE-03</t>
+  </si>
+  <si>
+    <t>EXE-TC-03</t>
+  </si>
+  <si>
+    <t>Chrome v145 /
+Windows 13</t>
+  </si>
+  <si>
+    <t>Verify system validates email format</t>
+  </si>
+  <si>
+    <t>Register with invalid email format</t>
+  </si>
+  <si>
+    <t>Error message “Email incorrect” displayed</t>
   </si>
 </sst>
 </file>
@@ -569,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A298028-139E-4333-8689-0C2300BF2C53}">
-  <dimension ref="D4:Q6"/>
+  <dimension ref="D4:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -724,6 +743,50 @@
         <v>26</v>
       </c>
     </row>
+    <row r="7" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="7">
+        <v>46076</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update TEST EXCETUION regist 4 #1
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F67A43C-4CBC-49A7-B5C0-79A086074F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6A62D0-41DA-446D-B9C9-E2C54F5ACAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EXE Regisration " sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>SUB</t>
   </si>
@@ -148,6 +148,25 @@
   </si>
   <si>
     <t>Error message “Email incorrect” displayed</t>
+  </si>
+  <si>
+    <t>EXE-04</t>
+  </si>
+  <si>
+    <t>EXE-TC-04</t>
+  </si>
+  <si>
+    <t>Chrome v145 /
+Windows 14</t>
+  </si>
+  <si>
+    <t>Verify minimum password length (8 characters)</t>
+  </si>
+  <si>
+    <t>Register with password less than 8 characters</t>
+  </si>
+  <si>
+    <t>Error message "Password must have 8 characters” displayed</t>
   </si>
 </sst>
 </file>
@@ -588,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A298028-139E-4333-8689-0C2300BF2C53}">
-  <dimension ref="D4:Q7"/>
+  <dimension ref="D4:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -602,9 +621,9 @@
     <col min="6" max="6" width="12.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="15" width="21" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21" style="6" bestFit="1" customWidth="1"/>
@@ -787,6 +806,50 @@
         <v>36</v>
       </c>
     </row>
+    <row r="8" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update TEST EXCETUION regist 4 #2
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6A62D0-41DA-446D-B9C9-E2C54F5ACAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FEF0A8-BF4F-4CA8-89AA-A497E070558E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
   <si>
     <t>SUB</t>
   </si>
@@ -167,6 +167,16 @@
   </si>
   <si>
     <t>Error message "Password must have 8 characters” displayed</t>
+  </si>
+  <si>
+    <t>EXE-TC-05</t>
+  </si>
+  <si>
+    <t>Chrome v145 /
+Windows 15</t>
+  </si>
+  <si>
+    <t>Register with exactly 8 characters password</t>
   </si>
 </sst>
 </file>
@@ -239,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -262,11 +272,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -291,6 +327,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -607,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A298028-139E-4333-8689-0C2300BF2C53}">
-  <dimension ref="D4:Q8"/>
+  <dimension ref="D4:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -807,10 +855,10 @@
       </c>
     </row>
     <row r="8" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="10" t="s">
         <v>43</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -850,7 +898,51 @@
         <v>42</v>
       </c>
     </row>
+    <row r="9" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D9" s="13"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D8:D9"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update TEST EXCETUION regist 5 #1
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FEF0A8-BF4F-4CA8-89AA-A497E070558E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A81426D-1A8D-4A6B-AB4B-56975EE874B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>SUB</t>
   </si>
@@ -169,6 +169,9 @@
     <t>Error message "Password must have 8 characters” displayed</t>
   </si>
   <si>
+    <t>EXE-05</t>
+  </si>
+  <si>
     <t>EXE-TC-05</t>
   </si>
   <si>
@@ -177,6 +180,29 @@
   </si>
   <si>
     <t>Register with exactly 8 characters password</t>
+  </si>
+  <si>
+    <t>EXE-TC-06</t>
+  </si>
+  <si>
+    <t>Chrome v145 /
+Windows 16</t>
+  </si>
+  <si>
+    <t>EXE-TC-07</t>
+  </si>
+  <si>
+    <t>Chrome v145 /
+Windows 17</t>
+  </si>
+  <si>
+    <t>Verify required fields cannot be empty</t>
+  </si>
+  <si>
+    <t>Register with empty email</t>
+  </si>
+  <si>
+    <t>Error message "You must proviled your email” displayed</t>
   </si>
 </sst>
 </file>
@@ -655,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A298028-139E-4333-8689-0C2300BF2C53}">
-  <dimension ref="D4:Q9"/>
+  <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -902,7 +928,7 @@
       <c r="D9" s="13"/>
       <c r="E9" s="11"/>
       <c r="F9" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>7</v>
@@ -911,7 +937,7 @@
         <v>40</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>9</v>
@@ -935,13 +961,99 @@
         <v>46077</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D10" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D11" s="13"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update TEST EXCETUION regist 5 #2
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A81426D-1A8D-4A6B-AB4B-56975EE874B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83AA4D8-8058-479C-8A97-F4E7B43B7396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
     <t>SUB</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>Error message "You must proviled your email” displayed</t>
+  </si>
+  <si>
+    <t>Fill email, leave password empty, click register</t>
+  </si>
+  <si>
+    <t>Error message "Password is required" displayed</t>
   </si>
 </sst>
 </file>
@@ -683,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A298028-139E-4333-8689-0C2300BF2C53}">
   <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -978,7 +984,7 @@
         <v>7</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>55</v>
@@ -1018,16 +1024,16 @@
         <v>7</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
update TEST EXCETUION regist 6
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83AA4D8-8058-479C-8A97-F4E7B43B7396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C66165-E251-4D01-81F4-3CC073A3FD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
   <si>
     <t>SUB</t>
   </si>
@@ -205,10 +205,29 @@
     <t>Error message "You must proviled your email” displayed</t>
   </si>
   <si>
+    <t>EXE-06</t>
+  </si>
+  <si>
     <t>Fill email, leave password empty, click register</t>
   </si>
   <si>
     <t>Error message "Password is required" displayed</t>
+  </si>
+  <si>
+    <t>EXE-TC-08</t>
+  </si>
+  <si>
+    <t>Chrome v145 /
+Windows 18</t>
+  </si>
+  <si>
+    <t>Verify user can login after successful registration</t>
+  </si>
+  <si>
+    <t>Login after successful registration</t>
+  </si>
+  <si>
+    <t>Login Successful</t>
   </si>
 </sst>
 </file>
@@ -687,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A298028-139E-4333-8689-0C2300BF2C53}">
-  <dimension ref="D4:Q11"/>
+  <dimension ref="D4:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1027,13 +1046,13 @@
         <v>46</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>22</v>
@@ -1052,6 +1071,50 @@
       </c>
       <c r="Q11" s="5" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update TEST EXCETUION login 1
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C66165-E251-4D01-81F4-3CC073A3FD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCC203F-E3FD-4392-BD2D-2B1F27191BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
   <sheets>
     <sheet name="EXE Regisration " sheetId="1" r:id="rId1"/>
+    <sheet name="EXE Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="69">
   <si>
     <t>SUB</t>
   </si>
@@ -228,6 +229,18 @@
   </si>
   <si>
     <t>Login Successful</t>
+  </si>
+  <si>
+    <t>Login Module</t>
+  </si>
+  <si>
+    <t>Verify user can login with valid email and password</t>
+  </si>
+  <si>
+    <t>Login with valid email and password</t>
+  </si>
+  <si>
+    <t>User successfully logged in</t>
   </si>
 </sst>
 </file>
@@ -708,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A298028-139E-4333-8689-0C2300BF2C53}">
   <dimension ref="D4:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1127,4 +1140,428 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8856AFAE-B501-4768-B0BD-28B339F7F269}">
+  <dimension ref="D4:Q12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="6"/>
+    <col min="4" max="4" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="21" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="4:17" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D9" s="13"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D10" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D11" s="13"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update TEST EXCETUION login 2
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCC203F-E3FD-4392-BD2D-2B1F27191BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920B285D-C320-484B-B369-F88BFFB6896B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="72">
   <si>
     <t>SUB</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>User successfully logged in</t>
+  </si>
+  <si>
+    <t>Verify system displays error when password is incorrect</t>
+  </si>
+  <si>
+    <t>Login with incorrect password</t>
+  </si>
+  <si>
+    <t>Error message “Password is incorect, please try again” displayed</t>
   </si>
 </sst>
 </file>
@@ -1146,21 +1155,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8856AFAE-B501-4768-B0BD-28B339F7F269}">
   <dimension ref="D4:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="6"/>
     <col min="4" max="4" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="54.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="58.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="15" width="21" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21" style="6" bestFit="1" customWidth="1"/>
@@ -1260,7 +1269,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>25</v>
@@ -1272,13 +1281,13 @@
         <v>24</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
update TEST EXCETUION login 3
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920B285D-C320-484B-B369-F88BFFB6896B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C4C2C3-D08D-460F-9289-B580B4BC1260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="80">
   <si>
     <t>SUB</t>
   </si>
@@ -138,6 +138,9 @@
     <t>EXE-TC-03</t>
   </si>
   <si>
+    <t>BUG-02</t>
+  </si>
+  <si>
     <t>Chrome v145 /
 Windows 13</t>
   </si>
@@ -222,6 +225,13 @@
 Windows 18</t>
   </si>
   <si>
+    <t>EXE-TC-09</t>
+  </si>
+  <si>
+    <t>Chrome v145 /
+Windows 19</t>
+  </si>
+  <si>
     <t>Verify user can login after successful registration</t>
   </si>
   <si>
@@ -250,6 +260,21 @@
   </si>
   <si>
     <t>Error message “Password is incorect, please try again” displayed</t>
+  </si>
+  <si>
+    <t>EXE-07</t>
+  </si>
+  <si>
+    <t>Verify error when email not registered</t>
+  </si>
+  <si>
+    <t>Login with unregistered email</t>
+  </si>
+  <si>
+    <t>Error message “Email and passwordincorrect” displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOW</t>
   </si>
 </sst>
 </file>
@@ -322,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -371,11 +396,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,6 +448,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -730,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A298028-139E-4333-8689-0C2300BF2C53}">
   <dimension ref="D4:Q12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -888,7 +930,7 @@
         <v>34</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>35</v>
@@ -900,13 +942,13 @@
         <v>34</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>22</v>
@@ -924,33 +966,33 @@
         <v>46076</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D8" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>22</v>
@@ -968,23 +1010,23 @@
         <v>46077</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D9" s="13"/>
       <c r="E9" s="11"/>
       <c r="F9" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>9</v>
@@ -1008,33 +1050,33 @@
         <v>46077</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D10" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>22</v>
@@ -1052,29 +1094,29 @@
         <v>46077</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D11" s="13"/>
       <c r="E11" s="11"/>
       <c r="F11" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>22</v>
@@ -1092,33 +1134,33 @@
         <v>46077</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>22</v>
@@ -1136,7 +1178,7 @@
         <v>46077</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1153,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8856AFAE-B501-4768-B0BD-28B339F7F269}">
-  <dimension ref="D4:Q12"/>
+  <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1225,25 +1267,25 @@
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>22</v>
@@ -1269,34 +1311,34 @@
         <v>24</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>31</v>
+        <v>74</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>20</v>
@@ -1313,34 +1355,34 @@
         <v>34</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>22</v>
+        <v>78</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>20</v>
@@ -1349,33 +1391,33 @@
         <v>46077</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D8" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="I8" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>22</v>
@@ -1393,23 +1435,23 @@
         <v>46077</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D9" s="13"/>
-      <c r="E9" s="11"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>9</v>
@@ -1433,33 +1475,29 @@
         <v>46077</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D10" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>54</v>
-      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="4" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>22</v>
@@ -1477,29 +1515,33 @@
         <v>46077</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D11" s="13"/>
-      <c r="E11" s="11"/>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="F11" s="4" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>22</v>
@@ -1514,63 +1556,18 @@
         <v>20</v>
       </c>
       <c r="P11" s="7">
-        <v>46077</v>
+        <v>46078</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P12" s="7">
-        <v>46077</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>61</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+  <mergeCells count="2">
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update TEST EXCETUION login 4 #1
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C4C2C3-D08D-460F-9289-B580B4BC1260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE5227D-34CB-4341-B206-C0A9A0905EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="83">
   <si>
     <t>SUB</t>
   </si>
@@ -275,6 +275,15 @@
   </si>
   <si>
     <t xml:space="preserve"> LOW</t>
+  </si>
+  <si>
+    <t>Verify required fields validation</t>
+  </si>
+  <si>
+    <t>Login with empty email</t>
+  </si>
+  <si>
+    <t>Error message "Please enter your email or username” displayed</t>
   </si>
 </sst>
 </file>
@@ -1197,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8856AFAE-B501-4768-B0BD-28B339F7F269}">
   <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1408,7 @@
         <v>41</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>42</v>
@@ -1411,13 +1420,13 @@
         <v>41</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>29</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
update TEST EXECUTION login 4 #2
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE5227D-34CB-4341-B206-C0A9A0905EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB1DCBF-71E0-4F57-901D-709CCE7245D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="85">
   <si>
     <t>SUB</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>Error message "Please enter your email or username” displayed</t>
+  </si>
+  <si>
+    <t>Login with empty password</t>
+  </si>
+  <si>
+    <t>Error message "Please enter your password” displayed</t>
   </si>
 </sst>
 </file>
@@ -1206,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8856AFAE-B501-4768-B0BD-28B339F7F269}">
   <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1460,13 +1466,13 @@
         <v>41</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
update TEST EXECUTION login 4 #3
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB1DCBF-71E0-4F57-901D-709CCE7245D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67584224-A538-406F-828D-1E716C346A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="87">
   <si>
     <t>SUB</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>Error message "Please enter your password” displayed</t>
+  </si>
+  <si>
+    <t>Login with both fields empty</t>
+  </si>
+  <si>
+    <t>Error message "Please enter your user and password” displayed</t>
   </si>
 </sst>
 </file>
@@ -1212,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8856AFAE-B501-4768-B0BD-28B339F7F269}">
   <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1506,13 +1512,13 @@
         <v>58</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
update TEST EXECUTION login 5
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67584224-A538-406F-828D-1E716C346A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D43E09-0B09-47DA-9866-CEBA4DD3D496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="88">
   <si>
     <t>SUB</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>Error message "Please enter your user and password” displayed</t>
+  </si>
+  <si>
+    <t>User already registered</t>
   </si>
 </sst>
 </file>
@@ -1218,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8856AFAE-B501-4768-B0BD-28B339F7F269}">
   <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1547,7 @@
         <v>47</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>63</v>
@@ -1559,7 +1562,7 @@
         <v>66</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
update TEST EXECUTION authorization
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D43E09-0B09-47DA-9866-CEBA4DD3D496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9B51FA-9D24-4899-A543-8A78A9E0ABB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
   <sheets>
     <sheet name="EXE Regisration " sheetId="1" r:id="rId1"/>
     <sheet name="EXE Login" sheetId="2" r:id="rId2"/>
+    <sheet name="EXE Authorization" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="88">
   <si>
     <t>SUB</t>
   </si>
@@ -1221,7 +1222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8856AFAE-B501-4768-B0BD-28B339F7F269}">
   <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="G4" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -1594,4 +1595,382 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E9E2AC-9BB7-495F-9DBA-96A9A36DE5E0}">
+  <dimension ref="D4:Q11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="6"/>
+    <col min="4" max="4" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="58.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="21" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="4:17" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D10" s="13"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" s="7">
+        <v>46078</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upload TEST EXECUTION logout 1
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9B51FA-9D24-4899-A543-8A78A9E0ABB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC7FB5C-8FE8-448F-AB79-0950ADDE5754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
   <sheets>
     <sheet name="EXE Regisration " sheetId="1" r:id="rId1"/>
     <sheet name="EXE Login" sheetId="2" r:id="rId2"/>
     <sheet name="EXE Authorization" sheetId="3" r:id="rId3"/>
+    <sheet name="EXE Logout" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="92">
   <si>
     <t>SUB</t>
   </si>
@@ -300,6 +301,18 @@
   </si>
   <si>
     <t>User already registered</t>
+  </si>
+  <si>
+    <t>Verify user can logout successfully</t>
+  </si>
+  <si>
+    <t>Logout Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logout after successful login </t>
+  </si>
+  <si>
+    <t>User successfully logged out</t>
   </si>
 </sst>
 </file>
@@ -463,22 +476,22 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -995,10 +1008,10 @@
       </c>
     </row>
     <row r="8" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="13" t="s">
         <v>44</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1039,8 +1052,8 @@
       </c>
     </row>
     <row r="9" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D9" s="13"/>
-      <c r="E9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="4" t="s">
         <v>48</v>
       </c>
@@ -1079,10 +1092,10 @@
       </c>
     </row>
     <row r="10" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="13" t="s">
         <v>55</v>
       </c>
       <c r="F10" s="4" t="s">
@@ -1123,8 +1136,8 @@
       </c>
     </row>
     <row r="11" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D11" s="13"/>
-      <c r="E11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="4" t="s">
         <v>53</v>
       </c>
@@ -1222,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8856AFAE-B501-4768-B0BD-28B339F7F269}">
   <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -1420,10 +1433,10 @@
       </c>
     </row>
     <row r="8" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="13" t="s">
         <v>80</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1464,8 +1477,8 @@
       </c>
     </row>
     <row r="9" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="4" t="s">
         <v>48</v>
       </c>
@@ -1504,8 +1517,8 @@
       </c>
     </row>
     <row r="10" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D10" s="13"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="4" t="s">
         <v>61</v>
       </c>
@@ -1601,7 +1614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E9E2AC-9BB7-495F-9DBA-96A9A36DE5E0}">
   <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -1799,10 +1812,10 @@
       </c>
     </row>
     <row r="8" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="13" t="s">
         <v>80</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1843,8 +1856,8 @@
       </c>
     </row>
     <row r="9" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="4" t="s">
         <v>48</v>
       </c>
@@ -1883,8 +1896,386 @@
       </c>
     </row>
     <row r="10" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D10" s="13"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" s="7">
+        <v>46078</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B4BE7AA-1C7B-4E8F-96EC-5C6CA3FD3BFD}">
+  <dimension ref="D4:Q11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="6"/>
+    <col min="4" max="4" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="58.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="21" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="4:17" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="7">
+        <v>46080</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D9" s="11"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="7">
+        <v>46077</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D10" s="12"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="4" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
upload TEST EXECUTION logout 2
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC7FB5C-8FE8-448F-AB79-0950ADDE5754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC898AEF-BCAD-4B8D-9BE5-8D9469BD0A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="96">
   <si>
     <t>SUB</t>
   </si>
@@ -313,6 +313,18 @@
   </si>
   <si>
     <t>User successfully logged out</t>
+  </si>
+  <si>
+    <t>Verify user cannot access restricted page after logout</t>
+  </si>
+  <si>
+    <t>Access resticted page after logout</t>
+  </si>
+  <si>
+    <t>User cannot access restricted page</t>
+  </si>
+  <si>
+    <t>User directed in login / register page</t>
   </si>
 </sst>
 </file>
@@ -1992,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B4BE7AA-1C7B-4E8F-96EC-5C6CA3FD3BFD}">
   <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2106,25 +2118,25 @@
         <v>24</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>29</v>
+        <v>93</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>22</v>
@@ -2139,229 +2151,14 @@
         <v>20</v>
       </c>
       <c r="P6" s="7">
-        <v>46077</v>
+        <v>46080</v>
       </c>
       <c r="Q6" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7" s="7">
-        <v>46077</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="7">
-        <v>46077</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D9" s="11"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P9" s="7">
-        <v>46077</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D10" s="12"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="7">
-        <v>46077</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P11" s="7">
-        <v>46078</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
+    <row r="11" spans="4:17" ht="31.5" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload TEST EXECUTION logout 3
</commit_message>
<xml_diff>
--- a/documentation/TEST EXECUTION.xlsx
+++ b/documentation/TEST EXECUTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC898AEF-BCAD-4B8D-9BE5-8D9469BD0A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AF8AC6-3607-4D6B-8BDE-415EDC62CC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{1DDAD4FE-2D96-4A5D-8208-8609A00B936D}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="99">
   <si>
     <t>SUB</t>
   </si>
@@ -325,6 +325,15 @@
   </si>
   <si>
     <t>User directed in login / register page</t>
+  </si>
+  <si>
+    <t>Verify user session is terminated after logout</t>
+  </si>
+  <si>
+    <t>Verify session is invalid after logout</t>
+  </si>
+  <si>
+    <t>User cannot access restricted paage after logout</t>
   </si>
 </sst>
 </file>
@@ -2004,8 +2013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B4BE7AA-1C7B-4E8F-96EC-5C6CA3FD3BFD}">
   <dimension ref="D4:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2157,8 +2166,53 @@
         <v>26</v>
       </c>
     </row>
+    <row r="7" spans="4:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="7">
+        <v>46081</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="11" spans="4:17" ht="31.5" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>